<commit_message>
update ignore and addin
</commit_message>
<xml_diff>
--- a/WebBrowser/bin/Release/data/smzdm.xlsx
+++ b/WebBrowser/bin/Release/data/smzdm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\smzdm\WebBrowser\bin\Release\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FADD2F4-41C7-430B-A209-E083FBDCD20D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEAB4A4-0A7F-48BF-873F-DCA47BE00C3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="85">
   <si>
     <t>phone</t>
   </si>
@@ -1171,7 +1171,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,7 +1453,7 @@
         <v>13</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>83</v>
@@ -1586,7 +1586,16 @@
         <v>13</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>12</v>
+        <v>80</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="L14" s="1">
         <v>1</v>
@@ -2056,7 +2065,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:H1048576 I1 I9">
+  <conditionalFormatting sqref="H1:H1048576 I1 H9:I9 I14">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
check in excel addin
</commit_message>
<xml_diff>
--- a/WebBrowser/bin/Release/data/smzdm.xlsx
+++ b/WebBrowser/bin/Release/data/smzdm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\smzdm\WebBrowser\bin\Release\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEAB4A4-0A7F-48BF-873F-DCA47BE00C3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22804CE-A1F0-4D5E-935A-29FA22F14CB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="88">
   <si>
     <t>phone</t>
   </si>
@@ -262,26 +262,35 @@
     <t>pages</t>
   </si>
   <si>
+    <t>ele</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>smzdm_share</t>
+  </si>
+  <si>
+    <t>50-56</t>
+  </si>
+  <si>
+    <t>computers</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>45-49</t>
+  </si>
+  <si>
     <t>y</t>
-  </si>
-  <si>
-    <t>ele</t>
-  </si>
-  <si>
-    <t>mode</t>
-  </si>
-  <si>
-    <t>smzdm_share</t>
-  </si>
-  <si>
-    <t>50-56</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +421,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -833,18 +848,42 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1171,7 +1210,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,7 +1222,8 @@
     <col min="7" max="7" width="16.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="37.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="1"/>
+    <col min="10" max="10" width="16.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
     <col min="12" max="12" width="25" style="1" customWidth="1"/>
     <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
@@ -1215,7 +1255,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>77</v>
@@ -1395,7 +1435,7 @@
         <v>13</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="L7" s="1">
         <v>1</v>
@@ -1453,16 +1493,16 @@
         <v>13</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L9" s="1">
         <v>1</v>
@@ -1560,7 +1600,16 @@
         <v>13</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>12</v>
+        <v>87</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="L13" s="1">
         <v>1</v>
@@ -1586,16 +1635,16 @@
         <v>13</v>
       </c>
       <c r="H14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="K14" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="L14" s="1">
         <v>1</v>
@@ -2065,15 +2114,21 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:H1048576 I1 H9:I9 I14">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="I1 H9:I9 H1:H1048576 I13:I14">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>n</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"r"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>